<commit_message>
changed 2nd layer limit to 200
</commit_message>
<xml_diff>
--- a/ftest/data/fm23/worked_example_policy_calculation_ri_test.xlsx
+++ b/ftest/data/fm23/worked_example_policy_calculation_ri_test.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ktest\ftest\data\fm23\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="12_ncr:500000_{B779528D-63AD-43A7-9022-A4D5CBC076C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12432" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Worked examples" sheetId="10" r:id="rId1"/>
@@ -220,7 +221,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
     <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* \-??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="_(* #,##0_);_(* \(#,##0\);_(* \-??_);_(@_)"/>
@@ -848,33 +849,34 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -884,6 +886,15 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="1" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -902,23 +913,13 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="20" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="22" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Comma 2" xfId="3"/>
+    <cellStyle name="Comma 2" xfId="3" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
     <cellStyle name="Percent" xfId="4" builtinId="5"/>
-    <cellStyle name="Percent 2" xfId="2"/>
+    <cellStyle name="Percent 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -1321,14 +1322,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:Q69"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15:E15"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47:N47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1547,26 +1548,26 @@
       <c r="B10" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="119">
+      <c r="C10" s="123">
         <v>100</v>
       </c>
-      <c r="D10" s="117"/>
-      <c r="E10" s="117"/>
-      <c r="F10" s="117">
+      <c r="D10" s="121"/>
+      <c r="E10" s="121"/>
+      <c r="F10" s="121">
         <v>100</v>
       </c>
-      <c r="G10" s="117"/>
-      <c r="H10" s="118"/>
-      <c r="I10" s="119">
+      <c r="G10" s="121"/>
+      <c r="H10" s="122"/>
+      <c r="I10" s="123">
         <v>100</v>
       </c>
-      <c r="J10" s="117"/>
-      <c r="K10" s="117"/>
-      <c r="L10" s="117">
+      <c r="J10" s="121"/>
+      <c r="K10" s="121"/>
+      <c r="L10" s="121">
         <v>100</v>
       </c>
-      <c r="M10" s="117"/>
-      <c r="N10" s="118"/>
+      <c r="M10" s="121"/>
+      <c r="N10" s="122"/>
       <c r="O10" s="23"/>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.3">
@@ -1597,22 +1598,22 @@
       <c r="B12" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="120">
+      <c r="C12" s="124">
         <v>10000</v>
       </c>
-      <c r="D12" s="121"/>
-      <c r="E12" s="121"/>
-      <c r="F12" s="121"/>
-      <c r="G12" s="121"/>
-      <c r="H12" s="122"/>
-      <c r="I12" s="120">
+      <c r="D12" s="125"/>
+      <c r="E12" s="125"/>
+      <c r="F12" s="125"/>
+      <c r="G12" s="125"/>
+      <c r="H12" s="126"/>
+      <c r="I12" s="124">
         <v>10000</v>
       </c>
-      <c r="J12" s="121"/>
-      <c r="K12" s="121"/>
-      <c r="L12" s="121"/>
-      <c r="M12" s="121"/>
-      <c r="N12" s="122"/>
+      <c r="J12" s="125"/>
+      <c r="K12" s="125"/>
+      <c r="L12" s="125"/>
+      <c r="M12" s="125"/>
+      <c r="N12" s="126"/>
       <c r="O12" s="27"/>
     </row>
     <row r="13" spans="1:17" x14ac:dyDescent="0.3">
@@ -1661,11 +1662,11 @@
         <v>40</v>
       </c>
       <c r="B15" s="19"/>
-      <c r="C15" s="105">
+      <c r="C15" s="112">
         <v>10</v>
       </c>
-      <c r="D15" s="106"/>
-      <c r="E15" s="106"/>
+      <c r="D15" s="107"/>
+      <c r="E15" s="107"/>
       <c r="F15" s="19"/>
       <c r="G15" s="19"/>
       <c r="H15" s="85"/>
@@ -1682,11 +1683,11 @@
         <v>41</v>
       </c>
       <c r="B16" s="19"/>
-      <c r="C16" s="105">
+      <c r="C16" s="112">
         <v>100</v>
       </c>
-      <c r="D16" s="106"/>
-      <c r="E16" s="106"/>
+      <c r="D16" s="107"/>
+      <c r="E16" s="107"/>
       <c r="F16" s="83"/>
       <c r="G16" s="83"/>
       <c r="H16" s="84"/>
@@ -1703,11 +1704,11 @@
         <v>42</v>
       </c>
       <c r="B17" s="19"/>
-      <c r="C17" s="105">
+      <c r="C17" s="112">
         <v>0.5</v>
       </c>
-      <c r="D17" s="106"/>
-      <c r="E17" s="106"/>
+      <c r="D17" s="107"/>
+      <c r="E17" s="107"/>
       <c r="F17" s="83"/>
       <c r="G17" s="83"/>
       <c r="H17" s="84"/>
@@ -1743,20 +1744,20 @@
         <v>54</v>
       </c>
       <c r="B19" s="19"/>
-      <c r="C19" s="105">
+      <c r="C19" s="112">
         <v>0</v>
       </c>
-      <c r="D19" s="106"/>
-      <c r="E19" s="106"/>
-      <c r="F19" s="106"/>
-      <c r="G19" s="106"/>
-      <c r="H19" s="106"/>
-      <c r="I19" s="106"/>
-      <c r="J19" s="106"/>
-      <c r="K19" s="106"/>
-      <c r="L19" s="106"/>
-      <c r="M19" s="106"/>
-      <c r="N19" s="109"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="107"/>
+      <c r="F19" s="107"/>
+      <c r="G19" s="107"/>
+      <c r="H19" s="107"/>
+      <c r="I19" s="107"/>
+      <c r="J19" s="107"/>
+      <c r="K19" s="107"/>
+      <c r="L19" s="107"/>
+      <c r="M19" s="107"/>
+      <c r="N19" s="108"/>
       <c r="O19" s="20"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -1764,20 +1765,20 @@
         <v>55</v>
       </c>
       <c r="B20" s="19"/>
-      <c r="C20" s="105">
+      <c r="C20" s="112">
         <v>100</v>
       </c>
-      <c r="D20" s="106"/>
-      <c r="E20" s="106"/>
-      <c r="F20" s="106"/>
-      <c r="G20" s="106"/>
-      <c r="H20" s="106"/>
-      <c r="I20" s="106"/>
-      <c r="J20" s="106"/>
-      <c r="K20" s="106"/>
-      <c r="L20" s="106"/>
-      <c r="M20" s="106"/>
-      <c r="N20" s="109"/>
+      <c r="D20" s="107"/>
+      <c r="E20" s="107"/>
+      <c r="F20" s="107"/>
+      <c r="G20" s="107"/>
+      <c r="H20" s="107"/>
+      <c r="I20" s="107"/>
+      <c r="J20" s="107"/>
+      <c r="K20" s="107"/>
+      <c r="L20" s="107"/>
+      <c r="M20" s="107"/>
+      <c r="N20" s="108"/>
       <c r="O20" s="20"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -1785,20 +1786,20 @@
         <v>56</v>
       </c>
       <c r="B21" s="19"/>
-      <c r="C21" s="110">
+      <c r="C21" s="106">
         <v>1</v>
       </c>
-      <c r="D21" s="106"/>
-      <c r="E21" s="106"/>
-      <c r="F21" s="106"/>
-      <c r="G21" s="106"/>
-      <c r="H21" s="106"/>
-      <c r="I21" s="106"/>
-      <c r="J21" s="106"/>
-      <c r="K21" s="106"/>
-      <c r="L21" s="106"/>
-      <c r="M21" s="106"/>
-      <c r="N21" s="109"/>
+      <c r="D21" s="107"/>
+      <c r="E21" s="107"/>
+      <c r="F21" s="107"/>
+      <c r="G21" s="107"/>
+      <c r="H21" s="107"/>
+      <c r="I21" s="107"/>
+      <c r="J21" s="107"/>
+      <c r="K21" s="107"/>
+      <c r="L21" s="107"/>
+      <c r="M21" s="107"/>
+      <c r="N21" s="108"/>
       <c r="O21" s="20"/>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -1806,20 +1807,20 @@
         <v>58</v>
       </c>
       <c r="B22" s="19"/>
-      <c r="C22" s="105">
+      <c r="C22" s="112">
         <v>100</v>
       </c>
-      <c r="D22" s="106"/>
-      <c r="E22" s="106"/>
-      <c r="F22" s="106"/>
-      <c r="G22" s="106"/>
-      <c r="H22" s="106"/>
-      <c r="I22" s="106"/>
-      <c r="J22" s="106"/>
-      <c r="K22" s="106"/>
-      <c r="L22" s="106"/>
-      <c r="M22" s="106"/>
-      <c r="N22" s="109"/>
+      <c r="D22" s="107"/>
+      <c r="E22" s="107"/>
+      <c r="F22" s="107"/>
+      <c r="G22" s="107"/>
+      <c r="H22" s="107"/>
+      <c r="I22" s="107"/>
+      <c r="J22" s="107"/>
+      <c r="K22" s="107"/>
+      <c r="L22" s="107"/>
+      <c r="M22" s="107"/>
+      <c r="N22" s="108"/>
       <c r="O22" s="20"/>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -1827,20 +1828,20 @@
         <v>59</v>
       </c>
       <c r="B23" s="19"/>
-      <c r="C23" s="105">
-        <v>100</v>
-      </c>
-      <c r="D23" s="106"/>
-      <c r="E23" s="106"/>
-      <c r="F23" s="106"/>
-      <c r="G23" s="106"/>
-      <c r="H23" s="106"/>
-      <c r="I23" s="106"/>
-      <c r="J23" s="106"/>
-      <c r="K23" s="106"/>
-      <c r="L23" s="106"/>
-      <c r="M23" s="106"/>
-      <c r="N23" s="109"/>
+      <c r="C23" s="112">
+        <v>200</v>
+      </c>
+      <c r="D23" s="107"/>
+      <c r="E23" s="107"/>
+      <c r="F23" s="107"/>
+      <c r="G23" s="107"/>
+      <c r="H23" s="107"/>
+      <c r="I23" s="107"/>
+      <c r="J23" s="107"/>
+      <c r="K23" s="107"/>
+      <c r="L23" s="107"/>
+      <c r="M23" s="107"/>
+      <c r="N23" s="108"/>
       <c r="O23" s="20"/>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -1848,20 +1849,20 @@
         <v>60</v>
       </c>
       <c r="B24" s="19"/>
-      <c r="C24" s="110">
+      <c r="C24" s="106">
         <v>0.5</v>
       </c>
-      <c r="D24" s="106"/>
-      <c r="E24" s="106"/>
-      <c r="F24" s="106"/>
-      <c r="G24" s="106"/>
-      <c r="H24" s="106"/>
-      <c r="I24" s="106"/>
-      <c r="J24" s="106"/>
-      <c r="K24" s="106"/>
-      <c r="L24" s="106"/>
-      <c r="M24" s="106"/>
-      <c r="N24" s="109"/>
+      <c r="D24" s="107"/>
+      <c r="E24" s="107"/>
+      <c r="F24" s="107"/>
+      <c r="G24" s="107"/>
+      <c r="H24" s="107"/>
+      <c r="I24" s="107"/>
+      <c r="J24" s="107"/>
+      <c r="K24" s="107"/>
+      <c r="L24" s="107"/>
+      <c r="M24" s="107"/>
+      <c r="N24" s="108"/>
       <c r="O24" s="20"/>
     </row>
     <row r="25" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -2050,30 +2051,30 @@
         <v>35</v>
       </c>
       <c r="B31" s="19"/>
-      <c r="C31" s="114">
+      <c r="C31" s="115">
         <f>SUM(C29:E29)</f>
         <v>200</v>
       </c>
-      <c r="D31" s="115"/>
-      <c r="E31" s="115"/>
-      <c r="F31" s="114">
+      <c r="D31" s="116"/>
+      <c r="E31" s="116"/>
+      <c r="F31" s="115">
         <f>SUM(F29:H29)</f>
         <v>200</v>
       </c>
-      <c r="G31" s="115"/>
-      <c r="H31" s="115"/>
-      <c r="I31" s="114">
+      <c r="G31" s="116"/>
+      <c r="H31" s="116"/>
+      <c r="I31" s="115">
         <f>SUM(I29:K29)</f>
         <v>200</v>
       </c>
-      <c r="J31" s="115"/>
-      <c r="K31" s="115"/>
-      <c r="L31" s="114">
+      <c r="J31" s="116"/>
+      <c r="K31" s="116"/>
+      <c r="L31" s="115">
         <f>SUM(L29:N29)</f>
         <v>200</v>
       </c>
-      <c r="M31" s="115"/>
-      <c r="N31" s="115"/>
+      <c r="M31" s="116"/>
+      <c r="N31" s="116"/>
       <c r="O31" s="35"/>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
@@ -2081,30 +2082,30 @@
         <v>36</v>
       </c>
       <c r="B32" s="19"/>
-      <c r="C32" s="111">
+      <c r="C32" s="109">
         <f>MIN(C31,C10)</f>
         <v>100</v>
       </c>
-      <c r="D32" s="112"/>
-      <c r="E32" s="112"/>
-      <c r="F32" s="111">
+      <c r="D32" s="110"/>
+      <c r="E32" s="110"/>
+      <c r="F32" s="109">
         <f>MIN(F31,F10)</f>
         <v>100</v>
       </c>
-      <c r="G32" s="112"/>
-      <c r="H32" s="112"/>
-      <c r="I32" s="111">
+      <c r="G32" s="110"/>
+      <c r="H32" s="110"/>
+      <c r="I32" s="109">
         <f>MIN(I31,I10)</f>
         <v>100</v>
       </c>
-      <c r="J32" s="112"/>
-      <c r="K32" s="112"/>
-      <c r="L32" s="111">
+      <c r="J32" s="110"/>
+      <c r="K32" s="110"/>
+      <c r="L32" s="109">
         <f>MIN(L31,L10)</f>
         <v>100</v>
       </c>
-      <c r="M32" s="112"/>
-      <c r="N32" s="112"/>
+      <c r="M32" s="110"/>
+      <c r="N32" s="110"/>
       <c r="O32" s="22"/>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.3">
@@ -2132,24 +2133,24 @@
         <v>37</v>
       </c>
       <c r="B34" s="19"/>
-      <c r="C34" s="123">
+      <c r="C34" s="118">
         <f>SUM(C32:H32)</f>
         <v>200</v>
       </c>
-      <c r="D34" s="124"/>
-      <c r="E34" s="124"/>
-      <c r="F34" s="124"/>
-      <c r="G34" s="124"/>
-      <c r="H34" s="125"/>
-      <c r="I34" s="123">
+      <c r="D34" s="119"/>
+      <c r="E34" s="119"/>
+      <c r="F34" s="119"/>
+      <c r="G34" s="119"/>
+      <c r="H34" s="120"/>
+      <c r="I34" s="118">
         <f>SUM(I32:N32)</f>
         <v>200</v>
       </c>
-      <c r="J34" s="124"/>
-      <c r="K34" s="124"/>
-      <c r="L34" s="124"/>
-      <c r="M34" s="124"/>
-      <c r="N34" s="125"/>
+      <c r="J34" s="119"/>
+      <c r="K34" s="119"/>
+      <c r="L34" s="119"/>
+      <c r="M34" s="119"/>
+      <c r="N34" s="120"/>
       <c r="O34" s="37"/>
       <c r="P34" s="38"/>
     </row>
@@ -2158,24 +2159,24 @@
         <v>38</v>
       </c>
       <c r="B35" s="19"/>
-      <c r="C35" s="111">
+      <c r="C35" s="109">
         <f>MIN(C34,C12)</f>
         <v>200</v>
       </c>
-      <c r="D35" s="112"/>
-      <c r="E35" s="112"/>
-      <c r="F35" s="112"/>
-      <c r="G35" s="112"/>
-      <c r="H35" s="113"/>
-      <c r="I35" s="111">
+      <c r="D35" s="110"/>
+      <c r="E35" s="110"/>
+      <c r="F35" s="110"/>
+      <c r="G35" s="110"/>
+      <c r="H35" s="111"/>
+      <c r="I35" s="109">
         <f>MIN(I34,I12)</f>
         <v>200</v>
       </c>
-      <c r="J35" s="112"/>
-      <c r="K35" s="112"/>
-      <c r="L35" s="112"/>
-      <c r="M35" s="112"/>
-      <c r="N35" s="113"/>
+      <c r="J35" s="110"/>
+      <c r="K35" s="110"/>
+      <c r="L35" s="110"/>
+      <c r="M35" s="110"/>
+      <c r="N35" s="111"/>
       <c r="O35" s="22"/>
       <c r="P35" s="38"/>
     </row>
@@ -2184,24 +2185,24 @@
         <v>22</v>
       </c>
       <c r="B36" s="19"/>
-      <c r="C36" s="111">
+      <c r="C36" s="109">
         <f>C35</f>
         <v>200</v>
       </c>
-      <c r="D36" s="112"/>
-      <c r="E36" s="112"/>
-      <c r="F36" s="112"/>
-      <c r="G36" s="112"/>
-      <c r="H36" s="113"/>
-      <c r="I36" s="111">
+      <c r="D36" s="110"/>
+      <c r="E36" s="110"/>
+      <c r="F36" s="110"/>
+      <c r="G36" s="110"/>
+      <c r="H36" s="111"/>
+      <c r="I36" s="109">
         <f>I35</f>
         <v>200</v>
       </c>
-      <c r="J36" s="112"/>
-      <c r="K36" s="112"/>
-      <c r="L36" s="112"/>
-      <c r="M36" s="112"/>
-      <c r="N36" s="113"/>
+      <c r="J36" s="110"/>
+      <c r="K36" s="110"/>
+      <c r="L36" s="110"/>
+      <c r="M36" s="110"/>
+      <c r="N36" s="111"/>
       <c r="O36" s="22"/>
       <c r="P36" s="38"/>
     </row>
@@ -2344,24 +2345,24 @@
         <v>48</v>
       </c>
       <c r="B40" s="19"/>
-      <c r="C40" s="114">
+      <c r="C40" s="115">
         <f>SUM(C38:E38)</f>
         <v>100</v>
       </c>
-      <c r="D40" s="115"/>
-      <c r="E40" s="115"/>
-      <c r="F40" s="114">
+      <c r="D40" s="116"/>
+      <c r="E40" s="116"/>
+      <c r="F40" s="115">
         <f>SUM(F38:N38)</f>
         <v>300</v>
       </c>
-      <c r="G40" s="115"/>
-      <c r="H40" s="115"/>
-      <c r="I40" s="115"/>
-      <c r="J40" s="115"/>
-      <c r="K40" s="115"/>
-      <c r="L40" s="115"/>
-      <c r="M40" s="115"/>
-      <c r="N40" s="116"/>
+      <c r="G40" s="116"/>
+      <c r="H40" s="116"/>
+      <c r="I40" s="116"/>
+      <c r="J40" s="116"/>
+      <c r="K40" s="116"/>
+      <c r="L40" s="116"/>
+      <c r="M40" s="116"/>
+      <c r="N40" s="117"/>
       <c r="O40" s="22">
         <f>O36</f>
         <v>0</v>
@@ -2373,23 +2374,23 @@
         <v>46</v>
       </c>
       <c r="B41" s="19"/>
-      <c r="C41" s="111">
+      <c r="C41" s="109">
         <f>C17*MIN(C16,MAX(C40-C15,0))</f>
         <v>45</v>
       </c>
-      <c r="D41" s="112"/>
-      <c r="E41" s="112"/>
-      <c r="F41" s="111">
+      <c r="D41" s="110"/>
+      <c r="E41" s="110"/>
+      <c r="F41" s="109">
         <v>0</v>
       </c>
-      <c r="G41" s="112"/>
-      <c r="H41" s="112"/>
-      <c r="I41" s="112"/>
-      <c r="J41" s="112"/>
-      <c r="K41" s="112"/>
-      <c r="L41" s="112"/>
-      <c r="M41" s="112"/>
-      <c r="N41" s="113"/>
+      <c r="G41" s="110"/>
+      <c r="H41" s="110"/>
+      <c r="I41" s="110"/>
+      <c r="J41" s="110"/>
+      <c r="K41" s="110"/>
+      <c r="L41" s="110"/>
+      <c r="M41" s="110"/>
+      <c r="N41" s="111"/>
       <c r="O41" s="22">
         <f>MIN(O40,O14)</f>
         <v>0</v>
@@ -2401,24 +2402,24 @@
         <v>52</v>
       </c>
       <c r="B42" s="19"/>
-      <c r="C42" s="111">
+      <c r="C42" s="109">
         <f>C40-C41</f>
         <v>55</v>
       </c>
-      <c r="D42" s="112"/>
-      <c r="E42" s="113"/>
-      <c r="F42" s="111">
+      <c r="D42" s="110"/>
+      <c r="E42" s="111"/>
+      <c r="F42" s="109">
         <f>F40-F41</f>
         <v>300</v>
       </c>
-      <c r="G42" s="112"/>
-      <c r="H42" s="112"/>
-      <c r="I42" s="112"/>
-      <c r="J42" s="112"/>
-      <c r="K42" s="112"/>
-      <c r="L42" s="112"/>
-      <c r="M42" s="112"/>
-      <c r="N42" s="113"/>
+      <c r="G42" s="110"/>
+      <c r="H42" s="110"/>
+      <c r="I42" s="110"/>
+      <c r="J42" s="110"/>
+      <c r="K42" s="110"/>
+      <c r="L42" s="110"/>
+      <c r="M42" s="110"/>
+      <c r="N42" s="111"/>
       <c r="O42" s="22"/>
       <c r="P42" s="38"/>
     </row>
@@ -2563,21 +2564,21 @@
         <v>50</v>
       </c>
       <c r="B46" s="48"/>
-      <c r="C46" s="107">
+      <c r="C46" s="113">
         <f>SUM(C44:N44)</f>
         <v>355</v>
       </c>
-      <c r="D46" s="108"/>
-      <c r="E46" s="108"/>
-      <c r="F46" s="108"/>
-      <c r="G46" s="108"/>
-      <c r="H46" s="108"/>
-      <c r="I46" s="108"/>
-      <c r="J46" s="108"/>
-      <c r="K46" s="108"/>
-      <c r="L46" s="108"/>
-      <c r="M46" s="108"/>
-      <c r="N46" s="108"/>
+      <c r="D46" s="114"/>
+      <c r="E46" s="114"/>
+      <c r="F46" s="114"/>
+      <c r="G46" s="114"/>
+      <c r="H46" s="114"/>
+      <c r="I46" s="114"/>
+      <c r="J46" s="114"/>
+      <c r="K46" s="114"/>
+      <c r="L46" s="114"/>
+      <c r="M46" s="114"/>
+      <c r="N46" s="114"/>
       <c r="O46" s="93"/>
       <c r="P46" s="103"/>
     </row>
@@ -2586,21 +2587,21 @@
         <v>51</v>
       </c>
       <c r="B47" s="19"/>
-      <c r="C47" s="105">
+      <c r="C47" s="112">
         <f>$C$21*MIN(C20,MAX(C46-C19))</f>
         <v>100</v>
       </c>
-      <c r="D47" s="106"/>
-      <c r="E47" s="106"/>
-      <c r="F47" s="106"/>
-      <c r="G47" s="106"/>
-      <c r="H47" s="106"/>
-      <c r="I47" s="106"/>
-      <c r="J47" s="106"/>
-      <c r="K47" s="106"/>
-      <c r="L47" s="106"/>
-      <c r="M47" s="106"/>
-      <c r="N47" s="106"/>
+      <c r="D47" s="107"/>
+      <c r="E47" s="107"/>
+      <c r="F47" s="107"/>
+      <c r="G47" s="107"/>
+      <c r="H47" s="107"/>
+      <c r="I47" s="107"/>
+      <c r="J47" s="107"/>
+      <c r="K47" s="107"/>
+      <c r="L47" s="107"/>
+      <c r="M47" s="107"/>
+      <c r="N47" s="107"/>
       <c r="P47" s="103"/>
     </row>
     <row r="48" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2608,21 +2609,21 @@
         <v>57</v>
       </c>
       <c r="B48" s="19"/>
-      <c r="C48" s="105">
+      <c r="C48" s="112">
         <f>C46-C47</f>
         <v>255</v>
       </c>
-      <c r="D48" s="106"/>
-      <c r="E48" s="106"/>
-      <c r="F48" s="106"/>
-      <c r="G48" s="106"/>
-      <c r="H48" s="106"/>
-      <c r="I48" s="106"/>
-      <c r="J48" s="106"/>
-      <c r="K48" s="106"/>
-      <c r="L48" s="106"/>
-      <c r="M48" s="106"/>
-      <c r="N48" s="106"/>
+      <c r="D48" s="107"/>
+      <c r="E48" s="107"/>
+      <c r="F48" s="107"/>
+      <c r="G48" s="107"/>
+      <c r="H48" s="107"/>
+      <c r="I48" s="107"/>
+      <c r="J48" s="107"/>
+      <c r="K48" s="107"/>
+      <c r="L48" s="107"/>
+      <c r="M48" s="107"/>
+      <c r="N48" s="107"/>
       <c r="P48" s="103"/>
     </row>
     <row r="49" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2744,21 +2745,21 @@
         <v>61</v>
       </c>
       <c r="B51" s="19"/>
-      <c r="C51" s="105">
+      <c r="C51" s="112">
         <f>$C$24*MIN($C$23,MAX($C$46-$C$22))</f>
-        <v>50</v>
-      </c>
-      <c r="D51" s="106"/>
-      <c r="E51" s="106"/>
-      <c r="F51" s="106"/>
-      <c r="G51" s="106"/>
-      <c r="H51" s="106"/>
-      <c r="I51" s="106"/>
-      <c r="J51" s="106"/>
-      <c r="K51" s="106"/>
-      <c r="L51" s="106"/>
-      <c r="M51" s="106"/>
-      <c r="N51" s="106"/>
+        <v>100</v>
+      </c>
+      <c r="D51" s="107"/>
+      <c r="E51" s="107"/>
+      <c r="F51" s="107"/>
+      <c r="G51" s="107"/>
+      <c r="H51" s="107"/>
+      <c r="I51" s="107"/>
+      <c r="J51" s="107"/>
+      <c r="K51" s="107"/>
+      <c r="L51" s="107"/>
+      <c r="M51" s="107"/>
+      <c r="N51" s="107"/>
       <c r="P51" s="103"/>
     </row>
     <row r="52" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2766,21 +2767,21 @@
         <v>62</v>
       </c>
       <c r="B52" s="19"/>
-      <c r="C52" s="105">
+      <c r="C52" s="112">
         <f>C48-C51</f>
-        <v>205</v>
-      </c>
-      <c r="D52" s="106"/>
-      <c r="E52" s="106"/>
-      <c r="F52" s="106"/>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
-      <c r="I52" s="106"/>
-      <c r="J52" s="106"/>
-      <c r="K52" s="106"/>
-      <c r="L52" s="106"/>
-      <c r="M52" s="106"/>
-      <c r="N52" s="106"/>
+        <v>155</v>
+      </c>
+      <c r="D52" s="107"/>
+      <c r="E52" s="107"/>
+      <c r="F52" s="107"/>
+      <c r="G52" s="107"/>
+      <c r="H52" s="107"/>
+      <c r="I52" s="107"/>
+      <c r="J52" s="107"/>
+      <c r="K52" s="107"/>
+      <c r="L52" s="107"/>
+      <c r="M52" s="107"/>
+      <c r="N52" s="107"/>
       <c r="P52" s="103"/>
     </row>
     <row r="53" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -2845,55 +2846,55 @@
       <c r="B54" s="102"/>
       <c r="C54" s="90">
         <f>C53*$C$52</f>
-        <v>15.880281690140844</v>
+        <v>12.007042253521126</v>
       </c>
       <c r="D54" s="91">
         <f t="shared" ref="D54:N54" si="13">D53*$C$52</f>
-        <v>7.9401408450704221</v>
+        <v>6.003521126760563</v>
       </c>
       <c r="E54" s="91">
         <f t="shared" si="13"/>
-        <v>7.9401408450704221</v>
+        <v>6.003521126760563</v>
       </c>
       <c r="F54" s="91">
         <f t="shared" si="13"/>
-        <v>28.87323943661972</v>
+        <v>21.83098591549296</v>
       </c>
       <c r="G54" s="91">
         <f t="shared" si="13"/>
-        <v>14.43661971830986</v>
+        <v>10.91549295774648</v>
       </c>
       <c r="H54" s="91">
         <f t="shared" si="13"/>
-        <v>14.43661971830986</v>
+        <v>10.91549295774648</v>
       </c>
       <c r="I54" s="91">
         <f t="shared" si="13"/>
-        <v>28.87323943661972</v>
+        <v>21.83098591549296</v>
       </c>
       <c r="J54" s="91">
         <f t="shared" si="13"/>
-        <v>14.43661971830986</v>
+        <v>10.91549295774648</v>
       </c>
       <c r="K54" s="91">
         <f t="shared" si="13"/>
-        <v>14.43661971830986</v>
+        <v>10.91549295774648</v>
       </c>
       <c r="L54" s="91">
         <f t="shared" si="13"/>
-        <v>28.87323943661972</v>
+        <v>21.83098591549296</v>
       </c>
       <c r="M54" s="91">
         <f t="shared" si="13"/>
-        <v>14.43661971830986</v>
+        <v>10.91549295774648</v>
       </c>
       <c r="N54" s="91">
         <f t="shared" si="13"/>
-        <v>14.43661971830986</v>
+        <v>10.91549295774648</v>
       </c>
       <c r="O54" s="104">
         <f>SUM(C54:N54)</f>
-        <v>204.99999999999997</v>
+        <v>155.00000000000006</v>
       </c>
     </row>
     <row r="55" spans="1:16" s="16" customFormat="1" x14ac:dyDescent="0.3">
@@ -3083,7 +3084,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -3121,7 +3122,7 @@
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" s="126" t="s">
+      <c r="A3" s="105" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>